<commit_message>
ER schema processing class and test
</commit_message>
<xml_diff>
--- a/data/abbreviations.xlsx
+++ b/data/abbreviations.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mandd/projects/DACKAR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A38059-EFE0-C246-987E-E4D65A124A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C0D59D-1944-CC41-A84A-338BF13ACA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52640" yWindow="6080" windowWidth="28800" windowHeight="18580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="abbreviations" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1288" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="1117">
   <si>
     <t>Full</t>
   </si>
@@ -3356,6 +3369,21 @@
   </si>
   <si>
     <t>breaker</t>
+  </si>
+  <si>
+    <t>s/d</t>
+  </si>
+  <si>
+    <t>s/b</t>
+  </si>
+  <si>
+    <t>stand-by</t>
+  </si>
+  <si>
+    <t>shut-down</t>
+  </si>
+  <si>
+    <t>vibe</t>
   </si>
 </sst>
 </file>
@@ -4222,11 +4250,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B644"/>
+  <dimension ref="A1:B647"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="224" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A633" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A645" sqref="A645"/>
+      <pane ySplit="1" topLeftCell="A632" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A648" sqref="A648"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9387,6 +9415,30 @@
         <v>1111</v>
       </c>
     </row>
+    <row r="645" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A645" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B645" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="646" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A646" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B646" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="647" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A647" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B647" t="s">
+        <v>1080</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B534">
     <sortCondition ref="A1:A534"/>

</xml_diff>